<commit_message>
further advances in csv. small tool
Small tool to access the files from old and new version.
</commit_message>
<xml_diff>
--- a/DeltaOldNew.xlsx
+++ b/DeltaOldNew.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Tabelle2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="352">
   <si>
     <t xml:space="preserve">Old</t>
   </si>
@@ -818,6 +819,264 @@
   </si>
   <si>
     <t xml:space="preserve">tentative_diagnosis_other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">farms_matched.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_ai_sink_sruveillance_sample_receiption_form_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formdata_AI_Sample_From_Ulo_Result.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_aqua_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formdata_AI_Sink_Surveillance.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_avian_influenza_investigate_p2_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formdata_AI_Sink_Surveillance_Result.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_avian_influenza_sample_p2_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formdata_AMR_Sink_Surveillance.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Declaration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_clinicalsign_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formdata_AMR_Sink_Surveillance_Result.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_data_collection_fisheries_list_antibiotics_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formdata_Avian_Influenza_Investigation.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_data_collection_fisheries_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formdata_Avian_Influenza_Sample.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_data_collection_petanimal_list_antibiotics_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formdata_Disease_Investigation.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_data_collection_petanimal_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_data_collection_poultry_list_antibiotics_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formdata_Participatory_Livestock_Assessment.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_data_collection_poultry_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_data_collection_ruminant_list_antibiotics_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">missing_farms.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_data_collection_ruminant_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_diagnosis_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_disease_determination_report_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_disease_investigation_p2_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_farm_assessment_closer_p2_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_farm_assessment_followup_p2_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_farm_assessment_p2_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_generic_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Decl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_lab_staff_name_entry_form_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_lab_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_medicine_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_participatory_livestock_assessment_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_patient_registrydyncsv_live_ear_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_patient_registrydyncsv_live_fecal_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_patient_registrydyncsv_live_parasite_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_patient_registrydyncsv_live_rapid_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_patient_registrydyncsv_live_skin_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_patient_registrydyncsv_live_urine_strip_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_patient_registrydyncsv_live_urine_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_pet_animal_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_poultry_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_rapid_kit_test_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_research_amr_data_mi_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_research_amr_data_poultry_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_rumenant_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_species_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_specimen_submission_collection_form_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_staff_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_status_sample_analysis_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_bahis_treatment_table.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_branch_catchment_area.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_database_static_script.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_datasource_definition.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_field_staffs.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_form_builder_forms.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_geo_data.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_geo_definition.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_list_definition.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_list_workflow.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_master_category.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_master_category_item.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_medicine.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_modulerolemap.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_module_catchment_area.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_module_definition.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_registered_device.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_rolewiseform.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_usermodule_branch.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_usermodule_menuitem.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_usermodule_menurolemap.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_usermodule_organizationrole.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_usermodule_organizations.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_usermodule_userbranchmap.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_usermodule_userfailedlogin.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_usermodule_usermoduleprofile.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_usermodule_userpasswordhistory.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_usermodule_userrolemap.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newbahis_xform_config_data.csv</t>
   </si>
 </sst>
 </file>
@@ -832,6 +1091,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -853,9 +1113,10 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -890,6 +1151,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD4EA6B"/>
         <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FFD4EA6B"/>
       </patternFill>
     </fill>
   </fills>
@@ -927,7 +1194,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -966,6 +1233,22 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1021,7 +1304,7 @@
       <rgbColor rgb="FFFFD7D7"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -1047,11 +1330,11 @@
   </sheetPr>
   <dimension ref="A1:M207"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="3" sqref="E39:G39 E41:G41 E43:G43 A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="1.52"/>
@@ -2332,4 +2615,960 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G73"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E43" activeCellId="2" sqref="E39:G39 E41:G41 E43:G43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="44.5078125" defaultRowHeight="14.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="73.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.78"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="11"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="C2" s="13" t="n">
+        <v>3160</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="G2" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="G3" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="C4" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="G4" s="13" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="G5" s="13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="G6" s="10" t="n">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="C7" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="G7" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" s="13" t="n">
+        <v>546</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="G8" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="C9" s="13" t="n">
+        <v>370</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="G9" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="C10" s="13" t="n">
+        <v>745</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="G10" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="13" t="n">
+        <v>3389</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="G11" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="C12" s="13" t="n">
+        <v>2866</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="G12" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="13" t="n">
+        <v>235179</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="G13" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="C14" s="13" t="n">
+        <v>754</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="G14" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E15" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="G15" s="10" t="n">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E16" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="G16" s="13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E17" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="G17" s="13" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E18" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="G18" s="13" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E19" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="G19" s="13" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E20" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="G20" s="13" t="n">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E21" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="G21" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E22" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="G22" s="10" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E23" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="G23" s="10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E24" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="G24" s="10" t="n">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E25" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="G25" s="13" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E26" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="G26" s="10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E27" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="G27" s="10" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E28" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="G28" s="10" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E29" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="G29" s="10" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E30" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="G30" s="10" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E31" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="10" t="n">
+        <v>11764</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E32" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="G32" s="10" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E33" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="G33" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E34" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="G34" s="13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E35" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="G35" s="13" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E36" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="G36" s="13" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F37" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G37" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F38" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="G38" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E39" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="G39" s="13" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E40" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="G40" s="10" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E41" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="G41" s="13" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E42" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="G42" s="10" t="n">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E43" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="G43" s="13" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E44" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="G44" s="10" t="n">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E45" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="G45" s="10" t="n">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E46" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="G46" s="10" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E47" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="G47" s="10" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E48" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="G48" s="10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E49" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="G49" s="10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E50" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G50" s="10" t="n">
+        <v>63625</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E51" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="G51" s="10" t="n">
+        <v>63625</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E52" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="G52" s="10" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E53" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="G53" s="10" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E54" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="G54" s="10" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E55" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="G55" s="10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E56" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="G56" s="10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E57" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="G57" s="10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E58" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="G58" s="10" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E59" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="G59" s="10" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E60" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="G60" s="10" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E61" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="G61" s="10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E62" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="G62" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E63" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="G63" s="10" t="n">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E64" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="G64" s="10" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E65" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="G65" s="10" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E66" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="G66" s="10" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E67" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="G67" s="10" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E68" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="G68" s="10" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E69" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="G69" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E70" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F70" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="G70" s="10" t="n">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E71" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F71" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="G71" s="10" t="n">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E72" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F72" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="G72" s="10" t="n">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E73" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F73" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="G73" s="10" t="n">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
first step towards mergind databases
bahis_dash changed only new file name with merged data
DeltaOldNew are some markers for the csv databases
loadnanalyse is a small code snipped to show csv files and column headers. Paths must be adjusted
prep_data is adjusted: species column is added and data from two sources, old and new is merged. !!!Sanity and db check is not made!!!
</commit_message>
<xml_diff>
--- a/DeltaOldNew.xlsx
+++ b/DeltaOldNew.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="373">
   <si>
     <t xml:space="preserve">Old</t>
   </si>
@@ -1080,6 +1080,9 @@
     <t xml:space="preserve">newbahis_xform_config_data.csv</t>
   </si>
   <si>
+    <t xml:space="preserve">Preped_data</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unnamed: 0</t>
   </si>
   <si>
@@ -1089,6 +1092,9 @@
     <t xml:space="preserve">10,11</t>
   </si>
   <si>
+    <t xml:space="preserve">!</t>
+  </si>
+  <si>
     <t xml:space="preserve">12,22</t>
   </si>
   <si>
@@ -1125,7 +1131,16 @@
     <t xml:space="preserve">34,13</t>
   </si>
   <si>
+    <t xml:space="preserve">Int</t>
+  </si>
+  <si>
     <t xml:space="preserve">35,16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Str</t>
+  </si>
+  <si>
+    <t xml:space="preserve">top_diagnosis</t>
   </si>
 </sst>
 </file>
@@ -1256,7 +1271,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1319,6 +1334,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -3865,16 +3884,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:F72"/>
+  <dimension ref="B1:I72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="14.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="35.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="16" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3884,6 +3904,9 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="I1" s="16" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E2" s="10" t="n">
@@ -3898,30 +3921,34 @@
         <v>0</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="D3" s="16"/>
+        <v>353</v>
+      </c>
+      <c r="D3" s="17"/>
       <c r="E3" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="15" t="s">
         <v>25</v>
       </c>
+      <c r="I3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="D4" s="16" t="n">
+      <c r="D4" s="17" t="n">
         <v>1.2</v>
       </c>
       <c r="E4" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="16" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3929,16 +3956,19 @@
       <c r="B5" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="16" t="n">
+      <c r="D5" s="17" t="n">
         <v>2.3</v>
       </c>
       <c r="E5" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3946,16 +3976,19 @@
       <c r="B6" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="16" t="n">
+      <c r="D6" s="17" t="n">
         <v>3.4</v>
       </c>
       <c r="E6" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="16" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3963,16 +3996,19 @@
       <c r="B7" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="16" t="n">
+      <c r="D7" s="17" t="n">
         <v>4.5</v>
       </c>
       <c r="E7" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="16" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3980,84 +4016,88 @@
       <c r="B8" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="16" t="n">
+      <c r="D8" s="17" t="n">
         <v>5.6</v>
       </c>
       <c r="E8" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="18" t="s">
         <v>35</v>
       </c>
+      <c r="I8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="D9" s="16" t="n">
+      <c r="D9" s="17" t="n">
         <v>6.7</v>
       </c>
       <c r="E9" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="18" t="s">
         <v>37</v>
       </c>
+      <c r="I9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="16" t="n">
+      <c r="D10" s="17" t="n">
         <v>7.8</v>
       </c>
       <c r="E10" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="18" t="s">
         <v>39</v>
       </c>
+      <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="16" t="n">
+      <c r="D11" s="17" t="n">
         <v>8.9</v>
       </c>
       <c r="E11" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="18" t="s">
         <v>41</v>
       </c>
+      <c r="I11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>353</v>
+      <c r="D12" s="17" t="s">
+        <v>354</v>
       </c>
       <c r="E12" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="18" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4065,17 +4105,20 @@
       <c r="B13" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>354</v>
+      <c r="D13" s="17" t="s">
+        <v>355</v>
       </c>
       <c r="E13" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="18" t="s">
         <v>45</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4085,7 +4128,7 @@
       <c r="C14" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="D14" s="16"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="10" t="n">
         <v>12</v>
       </c>
@@ -4100,13 +4143,13 @@
       <c r="C15" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="D15" s="16" t="s">
-        <v>355</v>
+      <c r="D15" s="17" t="s">
+        <v>357</v>
       </c>
       <c r="E15" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="15" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4117,8 +4160,8 @@
       <c r="C16" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>356</v>
+      <c r="D16" s="17" t="s">
+        <v>358</v>
       </c>
       <c r="E16" s="10" t="n">
         <v>14</v>
@@ -4134,8 +4177,8 @@
       <c r="C17" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="D17" s="16" t="s">
-        <v>357</v>
+      <c r="D17" s="17" t="s">
+        <v>359</v>
       </c>
       <c r="E17" s="10" t="n">
         <v>15</v>
@@ -4151,13 +4194,13 @@
       <c r="C18" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="D18" s="16" t="s">
-        <v>358</v>
+      <c r="D18" s="17" t="s">
+        <v>360</v>
       </c>
       <c r="E18" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="15" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4168,7 +4211,7 @@
       <c r="C19" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="D19" s="16"/>
+      <c r="D19" s="17"/>
       <c r="E19" s="10" t="n">
         <v>17</v>
       </c>
@@ -4183,7 +4226,7 @@
       <c r="C20" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="D20" s="16"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="10" t="n">
         <v>18</v>
       </c>
@@ -4198,7 +4241,7 @@
       <c r="C21" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="D21" s="16"/>
+      <c r="D21" s="17"/>
       <c r="E21" s="10" t="n">
         <v>19</v>
       </c>
@@ -4210,16 +4253,16 @@
       <c r="B22" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="D22" s="16" t="s">
-        <v>359</v>
+      <c r="D22" s="17" t="s">
+        <v>361</v>
       </c>
       <c r="E22" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="15" t="s">
         <v>63</v>
       </c>
     </row>
@@ -4227,16 +4270,16 @@
       <c r="B23" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="D23" s="16" t="s">
-        <v>360</v>
+      <c r="D23" s="17" t="s">
+        <v>362</v>
       </c>
       <c r="E23" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4247,7 +4290,7 @@
       <c r="C24" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="D24" s="16"/>
+      <c r="D24" s="17"/>
       <c r="E24" s="10" t="n">
         <v>22</v>
       </c>
@@ -4259,16 +4302,16 @@
       <c r="B25" s="10" t="n">
         <v>22</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="D25" s="16" t="s">
-        <v>361</v>
+      <c r="D25" s="17" t="s">
+        <v>363</v>
       </c>
       <c r="E25" s="10" t="n">
         <v>23</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="15" t="s">
         <v>69</v>
       </c>
     </row>
@@ -4276,16 +4319,16 @@
       <c r="B26" s="10" t="n">
         <v>23</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="D26" s="16" t="s">
-        <v>362</v>
+      <c r="D26" s="17" t="s">
+        <v>364</v>
       </c>
       <c r="E26" s="10" t="n">
         <v>24</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="15" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4293,16 +4336,19 @@
       <c r="B27" s="10" t="n">
         <v>24</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="D27" s="16" t="s">
-        <v>363</v>
+      <c r="D27" s="17" t="s">
+        <v>365</v>
       </c>
       <c r="E27" s="10" t="n">
         <v>25</v>
       </c>
       <c r="F27" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" s="16" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4310,16 +4356,19 @@
       <c r="B28" s="10" t="n">
         <v>25</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="16" t="s">
-        <v>364</v>
+      <c r="D28" s="17" t="s">
+        <v>366</v>
       </c>
       <c r="E28" s="10" t="n">
         <v>26</v>
       </c>
       <c r="F28" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="I28" s="16" t="s">
         <v>75</v>
       </c>
     </row>
@@ -4327,11 +4376,11 @@
       <c r="B29" s="10" t="n">
         <v>26</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="D29" s="16" t="s">
-        <v>365</v>
+      <c r="D29" s="17" t="s">
+        <v>367</v>
       </c>
       <c r="E29" s="10" t="n">
         <v>27</v>
@@ -4339,6 +4388,7 @@
       <c r="F29" s="13" t="s">
         <v>77</v>
       </c>
+      <c r="I29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="10" t="n">
@@ -4347,11 +4397,11 @@
       <c r="C30" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="D30" s="16"/>
+      <c r="D30" s="17"/>
       <c r="E30" s="10" t="n">
         <v>28</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="15" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4362,7 +4412,7 @@
       <c r="C31" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="D31" s="16"/>
+      <c r="D31" s="17"/>
       <c r="E31" s="10" t="n">
         <v>29</v>
       </c>
@@ -4377,7 +4427,7 @@
       <c r="C32" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="D32" s="16"/>
+      <c r="D32" s="17"/>
       <c r="E32" s="10" t="n">
         <v>30</v>
       </c>
@@ -4392,7 +4442,7 @@
       <c r="C33" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="D33" s="16"/>
+      <c r="D33" s="17"/>
       <c r="E33" s="10" t="n">
         <v>31</v>
       </c>
@@ -4407,7 +4457,7 @@
       <c r="C34" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="D34" s="16"/>
+      <c r="D34" s="17"/>
       <c r="E34" s="10" t="n">
         <v>32</v>
       </c>
@@ -4422,7 +4472,7 @@
       <c r="C35" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="D35" s="16"/>
+      <c r="D35" s="17"/>
       <c r="E35" s="10" t="n">
         <v>33</v>
       </c>
@@ -4437,7 +4487,7 @@
       <c r="C36" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="D36" s="16"/>
+      <c r="D36" s="17"/>
       <c r="E36" s="10" t="n">
         <v>34</v>
       </c>
@@ -4449,16 +4499,22 @@
       <c r="B37" s="10" t="n">
         <v>34</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="D37" s="16" t="s">
-        <v>366</v>
+      <c r="D37" s="17" t="s">
+        <v>368</v>
       </c>
       <c r="E37" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="I37" s="16" t="s">
         <v>93</v>
       </c>
     </row>
@@ -4466,17 +4522,23 @@
       <c r="B38" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="D38" s="16" t="s">
-        <v>367</v>
+      <c r="D38" s="17" t="s">
+        <v>370</v>
       </c>
       <c r="E38" s="10" t="n">
         <v>36</v>
       </c>
       <c r="F38" s="10" t="s">
         <v>95</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="I38" s="16" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4486,13 +4548,14 @@
       <c r="C39" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="D39" s="16"/>
+      <c r="D39" s="17"/>
       <c r="E39" s="10" t="n">
         <v>37</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>97</v>
       </c>
+      <c r="I39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="10" t="n">
@@ -4501,13 +4564,14 @@
       <c r="C40" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="D40" s="16"/>
+      <c r="D40" s="17"/>
       <c r="E40" s="10" t="n">
         <v>38</v>
       </c>
       <c r="F40" s="10" t="s">
         <v>99</v>
       </c>
+      <c r="I40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="10" t="n">
@@ -4516,7 +4580,7 @@
       <c r="C41" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="D41" s="16"/>
+      <c r="D41" s="17"/>
       <c r="E41" s="10" t="n">
         <v>39</v>
       </c>
@@ -4531,13 +4595,14 @@
       <c r="C42" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="D42" s="16"/>
+      <c r="D42" s="17"/>
       <c r="E42" s="10" t="n">
         <v>40</v>
       </c>
       <c r="F42" s="10" t="s">
         <v>103</v>
       </c>
+      <c r="I42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="10" t="n">
@@ -4546,7 +4611,7 @@
       <c r="C43" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="D43" s="16"/>
+      <c r="D43" s="17"/>
       <c r="E43" s="10" t="n">
         <v>41</v>
       </c>
@@ -4561,7 +4626,7 @@
       <c r="C44" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="D44" s="16"/>
+      <c r="D44" s="17"/>
       <c r="E44" s="10" t="n">
         <v>42</v>
       </c>
@@ -4576,7 +4641,7 @@
       <c r="C45" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="D45" s="16"/>
+      <c r="D45" s="17"/>
       <c r="E45" s="10" t="n">
         <v>43</v>
       </c>
@@ -4591,7 +4656,7 @@
       <c r="C46" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="D46" s="16"/>
+      <c r="D46" s="17"/>
       <c r="E46" s="10" t="n">
         <v>44</v>
       </c>
@@ -4606,7 +4671,7 @@
       <c r="C47" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="D47" s="16"/>
+      <c r="D47" s="17"/>
       <c r="E47" s="10" t="n">
         <v>45</v>
       </c>
@@ -4621,7 +4686,7 @@
       <c r="C48" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="D48" s="16"/>
+      <c r="D48" s="17"/>
       <c r="E48" s="10" t="n">
         <v>46</v>
       </c>
@@ -4636,7 +4701,7 @@
       <c r="C49" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="D49" s="16"/>
+      <c r="D49" s="17"/>
       <c r="E49" s="10" t="n">
         <v>47</v>
       </c>
@@ -4651,7 +4716,7 @@
       <c r="C50" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="D50" s="16"/>
+      <c r="D50" s="17"/>
       <c r="E50" s="10" t="n">
         <v>48</v>
       </c>
@@ -4666,7 +4731,7 @@
       <c r="C51" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="D51" s="16"/>
+      <c r="D51" s="17"/>
       <c r="E51" s="10" t="n">
         <v>49</v>
       </c>
@@ -4681,7 +4746,7 @@
       <c r="C52" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="D52" s="16"/>
+      <c r="D52" s="17"/>
       <c r="E52" s="10" t="n">
         <v>50</v>
       </c>
@@ -4696,7 +4761,7 @@
       <c r="C53" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="D53" s="16"/>
+      <c r="D53" s="17"/>
       <c r="E53" s="10" t="n">
         <v>51</v>
       </c>
@@ -4711,7 +4776,7 @@
       <c r="C54" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="D54" s="16"/>
+      <c r="D54" s="17"/>
       <c r="E54" s="10" t="n">
         <v>52</v>
       </c>
@@ -4726,7 +4791,7 @@
       <c r="C55" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="D55" s="16"/>
+      <c r="D55" s="17"/>
       <c r="E55" s="10" t="n">
         <v>53</v>
       </c>
@@ -4741,7 +4806,7 @@
       <c r="C56" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="D56" s="16"/>
+      <c r="D56" s="17"/>
       <c r="E56" s="10" t="n">
         <v>54</v>
       </c>
@@ -4756,7 +4821,7 @@
       <c r="C57" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="D57" s="16"/>
+      <c r="D57" s="17"/>
       <c r="E57" s="10" t="n">
         <v>55</v>
       </c>
@@ -4771,7 +4836,7 @@
       <c r="C58" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="D58" s="16"/>
+      <c r="D58" s="17"/>
     </row>
     <row r="59" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="10" t="n">
@@ -4780,7 +4845,7 @@
       <c r="C59" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="D59" s="16"/>
+      <c r="D59" s="17"/>
     </row>
     <row r="60" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="10" t="n">
@@ -4789,7 +4854,7 @@
       <c r="C60" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="D60" s="16"/>
+      <c r="D60" s="17"/>
     </row>
     <row r="61" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="10" t="n">
@@ -4798,7 +4863,7 @@
       <c r="C61" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="D61" s="16"/>
+      <c r="D61" s="17"/>
     </row>
     <row r="62" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="10" t="n">

</xml_diff>